<commit_message>
https://github.com/kwapisiewicz/MyBudget/issues/22 Inplemented logic for Card loading Adjusted testcases
</commit_message>
<xml_diff>
--- a/MyBudget.OperationsLoading.Tests/Resources/BNP_TestOperations.xlsx
+++ b/MyBudget.OperationsLoading.Tests/Resources/BNP_TestOperations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gniady\Source\Repos\MyBudget\MyBudget.OperationsLoading.Tests\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{298A4FDF-8762-440D-ACEF-7B64788B6C9F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2E49603-BE17-43B2-A19F-EE5E7A0EE734}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-2820" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ExcelExportFile" sheetId="1" r:id="rId1"/>
@@ -610,7 +610,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMK11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -697,7 +699,7 @@
     </row>
     <row r="3" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
-        <v>43885</v>
+        <v>43884</v>
       </c>
       <c r="B3" s="5">
         <v>43885</v>

</xml_diff>